<commit_message>
Horizontal/Vertical changed to Normalized/Denormalized with additional changes, initial draft
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_EC.xlsx
+++ b/curation/draft/collection/collection_specialization_EC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105B9B09-4707-43C3-B106-57429A716C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2C79ED-B6C3-E747-A503-E7A00DC41DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_EC" sheetId="1" r:id="rId1"/>
@@ -412,9 +412,6 @@
     <t>C48524</t>
   </si>
   <si>
-    <t>Number of 25-cm2 patches prescribed/day</t>
-  </si>
-  <si>
     <t>Study Drug</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>LZZT - 360i PoC 50cm2</t>
   </si>
   <si>
-    <t>Number of 50-cm2 patches prescribed/day</t>
-  </si>
-  <si>
     <t>ECDOSE</t>
   </si>
   <si>
@@ -434,6 +428,12 @@
   </si>
   <si>
     <t>C117479</t>
+  </si>
+  <si>
+    <t>Number of 25cm2 patches prescribed/day</t>
+  </si>
+  <si>
+    <t>Number of 50cm2 patches prescribed/day</t>
   </si>
 </sst>
 </file>
@@ -848,32 +848,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA16" sqref="AA16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="29" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="5"/>
-    <col min="8" max="8" width="38.140625" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="31.140625" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" customWidth="1"/>
-    <col min="13" max="13" width="25.85546875" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" customWidth="1"/>
-    <col min="16" max="16" width="31.140625" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="38.1640625" customWidth="1"/>
+    <col min="10" max="10" width="23.5" customWidth="1"/>
+    <col min="11" max="11" width="31.1640625" customWidth="1"/>
+    <col min="12" max="12" width="26.5" customWidth="1"/>
+    <col min="13" max="13" width="25.83203125" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" customWidth="1"/>
+    <col min="16" max="16" width="31.1640625" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" customWidth="1"/>
     <col min="25" max="25" width="22" style="3" customWidth="1"/>
-    <col min="26" max="26" width="30.42578125" style="3" customWidth="1"/>
-    <col min="27" max="27" width="15.7109375" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" customWidth="1"/>
+    <col min="26" max="26" width="30.5" style="3" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" customWidth="1"/>
+    <col min="28" max="28" width="16.5" customWidth="1"/>
     <col min="31" max="31" width="26" customWidth="1"/>
     <col min="32" max="32" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,7 +974,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>111</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>111</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>39</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>39</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>39</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>39</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>39</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>39</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>39</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>39</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>39</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>39</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>126</v>
       </c>
       <c r="J18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K18" t="s">
         <v>90</v>
@@ -1894,7 +1894,7 @@
         <v>43</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q18">
         <v>1</v>
@@ -1921,7 +1921,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>39</v>
       </c>
@@ -1941,22 +1941,22 @@
         <v>126</v>
       </c>
       <c r="J19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K19" t="s">
         <v>90</v>
       </c>
       <c r="L19" t="s">
+        <v>132</v>
+      </c>
+      <c r="M19" t="s">
+        <v>132</v>
+      </c>
+      <c r="N19" t="s">
         <v>134</v>
       </c>
-      <c r="M19" t="s">
-        <v>134</v>
-      </c>
-      <c r="N19" t="s">
-        <v>136</v>
-      </c>
       <c r="P19" s="3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="Q19">
         <v>2</v>
@@ -1965,19 +1965,19 @@
         <v>38</v>
       </c>
       <c r="S19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T19">
         <v>2</v>
       </c>
       <c r="AD19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AE19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>39</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>126</v>
       </c>
       <c r="J20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K20" t="s">
         <v>90</v>
@@ -2045,7 +2045,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>39</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>126</v>
       </c>
       <c r="J21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K21" t="s">
         <v>90</v>
@@ -2116,7 +2116,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>126</v>
       </c>
       <c r="J22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K22" t="s">
         <v>90</v>
@@ -2187,7 +2187,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>39</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>126</v>
       </c>
       <c r="J23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K23" t="s">
         <v>90</v>
@@ -2258,7 +2258,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>126</v>
       </c>
       <c r="J24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K24" t="s">
         <v>90</v>
@@ -2317,7 +2317,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>126</v>
       </c>
       <c r="J25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K25" t="s">
         <v>90</v>
@@ -2379,7 +2379,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>39</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>126</v>
       </c>
       <c r="J26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K26" t="s">
         <v>90</v>
@@ -2435,7 +2435,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>126</v>
       </c>
       <c r="J27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K27" t="s">
         <v>90</v>
@@ -2491,7 +2491,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>39</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>127</v>
       </c>
       <c r="J28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K28" t="s">
         <v>90</v>
@@ -2526,7 +2526,7 @@
         <v>43</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q28">
         <v>1</v>
@@ -2553,7 +2553,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31" ht="32" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>39</v>
       </c>
@@ -2573,22 +2573,22 @@
         <v>127</v>
       </c>
       <c r="J29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K29" t="s">
         <v>90</v>
       </c>
       <c r="L29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M29" t="s">
+        <v>132</v>
+      </c>
+      <c r="N29" t="s">
         <v>134</v>
       </c>
-      <c r="M29" t="s">
-        <v>134</v>
-      </c>
-      <c r="N29" t="s">
+      <c r="P29" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="Q29">
         <v>2</v>
@@ -2597,19 +2597,19 @@
         <v>38</v>
       </c>
       <c r="S29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T29">
         <v>2</v>
       </c>
       <c r="AD29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AE29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>39</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>127</v>
       </c>
       <c r="J30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K30" t="s">
         <v>90</v>
@@ -2677,7 +2677,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>127</v>
       </c>
       <c r="J31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K31" t="s">
         <v>90</v>
@@ -2748,7 +2748,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>39</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>127</v>
       </c>
       <c r="J32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K32" t="s">
         <v>90</v>
@@ -2819,7 +2819,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>39</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>127</v>
       </c>
       <c r="J33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K33" t="s">
         <v>90</v>
@@ -2890,7 +2890,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>39</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>127</v>
       </c>
       <c r="J34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K34" t="s">
         <v>90</v>
@@ -2949,7 +2949,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>39</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>127</v>
       </c>
       <c r="J35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K35" t="s">
         <v>90</v>
@@ -3011,7 +3011,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>39</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>127</v>
       </c>
       <c r="J36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K36" t="s">
         <v>90</v>
@@ -3067,7 +3067,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:31" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>39</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>127</v>
       </c>
       <c r="J37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K37" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
Update collections yamls and scripts (categories, derivations)
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_EC.xlsx
+++ b/curation/draft/collection/collection_specialization_EC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279B5781-A599-454D-8268-87D4D84D1772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCF6034-654E-44A6-AFEF-992D226A2B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_EC" sheetId="1" r:id="rId1"/>
@@ -863,33 +863,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="29" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="5"/>
-    <col min="8" max="8" width="38.1640625" customWidth="1"/>
-    <col min="10" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="31.1640625" customWidth="1"/>
-    <col min="13" max="13" width="26.5" customWidth="1"/>
-    <col min="14" max="14" width="25.83203125" customWidth="1"/>
-    <col min="16" max="16" width="20.83203125" customWidth="1"/>
-    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.796875" style="5"/>
+    <col min="8" max="8" width="38.1328125" customWidth="1"/>
+    <col min="10" max="10" width="23.46484375" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="31.1328125" customWidth="1"/>
+    <col min="13" max="13" width="26.46484375" customWidth="1"/>
+    <col min="14" max="14" width="25.796875" customWidth="1"/>
+    <col min="16" max="16" width="20.796875" customWidth="1"/>
+    <col min="17" max="17" width="31.1328125" customWidth="1"/>
     <col min="23" max="25" width="16.6640625" customWidth="1"/>
     <col min="28" max="28" width="22" style="3" customWidth="1"/>
-    <col min="29" max="29" width="30.5" style="3" customWidth="1"/>
+    <col min="29" max="29" width="30.46484375" style="3" customWidth="1"/>
     <col min="30" max="30" width="15.6640625" customWidth="1"/>
-    <col min="31" max="31" width="16.5" customWidth="1"/>
+    <col min="31" max="31" width="16.46484375" customWidth="1"/>
     <col min="34" max="34" width="26" customWidth="1"/>
     <col min="35" max="35" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>139</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -999,7 +999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="s">
         <v>109</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
         <v>109</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>39</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>39</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>39</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>39</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>39</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>39</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>39</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:34" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>39</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>39</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="J18" t="s">
         <v>131</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="5">
         <v>360</v>
       </c>
       <c r="L18" t="s">
@@ -1994,7 +1994,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>39</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="J19" t="s">
         <v>131</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="5">
         <v>360</v>
       </c>
       <c r="L19" t="s">
@@ -2056,7 +2056,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>39</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="J20" t="s">
         <v>131</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="5">
         <v>360</v>
       </c>
       <c r="L20" t="s">
@@ -2130,7 +2130,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>39</v>
       </c>
@@ -2155,7 +2155,7 @@
       <c r="J21" t="s">
         <v>131</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="5">
         <v>360</v>
       </c>
       <c r="L21" t="s">
@@ -2207,7 +2207,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="J22" t="s">
         <v>131</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="5">
         <v>360</v>
       </c>
       <c r="L22" t="s">
@@ -2284,7 +2284,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>39</v>
       </c>
@@ -2309,7 +2309,7 @@
       <c r="J23" t="s">
         <v>131</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="5">
         <v>360</v>
       </c>
       <c r="L23" t="s">
@@ -2361,7 +2361,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="J24" t="s">
         <v>131</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="5">
         <v>360</v>
       </c>
       <c r="L24" t="s">
@@ -2426,7 +2426,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -2451,7 +2451,7 @@
       <c r="J25" t="s">
         <v>131</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="5">
         <v>360</v>
       </c>
       <c r="L25" t="s">
@@ -2494,7 +2494,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>39</v>
       </c>
@@ -2519,7 +2519,7 @@
       <c r="J26" t="s">
         <v>131</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="5">
         <v>360</v>
       </c>
       <c r="L26" t="s">
@@ -2556,7 +2556,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="J27" t="s">
         <v>131</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="5">
         <v>360</v>
       </c>
       <c r="L27" t="s">
@@ -2618,7 +2618,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>39</v>
       </c>
@@ -2643,7 +2643,7 @@
       <c r="J28" t="s">
         <v>132</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="5">
         <v>360</v>
       </c>
       <c r="L28" t="s">
@@ -2686,7 +2686,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>39</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="J29" t="s">
         <v>132</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="5">
         <v>360</v>
       </c>
       <c r="L29" t="s">
@@ -2748,7 +2748,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>39</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="J30" t="s">
         <v>132</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="5">
         <v>360</v>
       </c>
       <c r="L30" t="s">
@@ -2822,7 +2822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="J31" t="s">
         <v>132</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="5">
         <v>360</v>
       </c>
       <c r="L31" t="s">
@@ -2899,7 +2899,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>39</v>
       </c>
@@ -2924,7 +2924,7 @@
       <c r="J32" t="s">
         <v>132</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="5">
         <v>360</v>
       </c>
       <c r="L32" t="s">
@@ -2976,7 +2976,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>39</v>
       </c>
@@ -3001,7 +3001,7 @@
       <c r="J33" t="s">
         <v>132</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="5">
         <v>360</v>
       </c>
       <c r="L33" t="s">
@@ -3053,7 +3053,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>39</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="J34" t="s">
         <v>132</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="5">
         <v>360</v>
       </c>
       <c r="L34" t="s">
@@ -3118,7 +3118,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>39</v>
       </c>
@@ -3143,7 +3143,7 @@
       <c r="J35" t="s">
         <v>132</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="5">
         <v>360</v>
       </c>
       <c r="L35" t="s">
@@ -3186,7 +3186,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>39</v>
       </c>
@@ -3211,7 +3211,7 @@
       <c r="J36" t="s">
         <v>132</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="5">
         <v>360</v>
       </c>
       <c r="L36" t="s">
@@ -3248,7 +3248,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>39</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="J37" t="s">
         <v>132</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="5">
         <v>360</v>
       </c>
       <c r="L37" t="s">

</xml_diff>